<commit_message>
ajuste: corrigindo as categorias
</commit_message>
<xml_diff>
--- a/analysis_Campinas/campinas_datasus/cps2010_dt_c.xlsx
+++ b/analysis_Campinas/campinas_datasus/cps2010_dt_c.xlsx
@@ -1,94 +1,101 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\dissertacao_etapa1\analysis_Campinas\campinas_datasus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C2F9C3-7B83-411D-A9B3-AD7CE8D2427F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t xml:space="preserve">cid_grupos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 a 4 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 a 9 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 a 14 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 a 19 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 a 24 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 a 29 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 a 34 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 a 39 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 a 44 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45 a 49 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 a 54 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55 a 59 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 a 64 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65 a 69 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70 a 74 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75 a 79 anos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80 anos e mais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doenças do aparelho circulatório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doenças do aparelho geniturinário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doenças do aparelho respiratório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doenças endócrinas, nutricionais e metabólicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neoplasmas</t>
+    <t>cid_grupos</t>
+  </si>
+  <si>
+    <t>0 a 4 anos</t>
+  </si>
+  <si>
+    <t>5 a 9 anos</t>
+  </si>
+  <si>
+    <t>10 a 14 anos</t>
+  </si>
+  <si>
+    <t>15 a 19 anos</t>
+  </si>
+  <si>
+    <t>20 a 24 anos</t>
+  </si>
+  <si>
+    <t>25 a 29 anos</t>
+  </si>
+  <si>
+    <t>30 a 34 anos</t>
+  </si>
+  <si>
+    <t>35 a 39 anos</t>
+  </si>
+  <si>
+    <t>40 a 44 anos</t>
+  </si>
+  <si>
+    <t>45 a 49 anos</t>
+  </si>
+  <si>
+    <t>50 a 54 anos</t>
+  </si>
+  <si>
+    <t>55 a 59 anos</t>
+  </si>
+  <si>
+    <t>60 a 64 anos</t>
+  </si>
+  <si>
+    <t>65 a 69 anos</t>
+  </si>
+  <si>
+    <t>70 a 74 anos</t>
+  </si>
+  <si>
+    <t>75 a 79 anos</t>
+  </si>
+  <si>
+    <t>80 anos e mais</t>
+  </si>
+  <si>
+    <t>Doenças do aparelho circulatório</t>
+  </si>
+  <si>
+    <t>Doenças do aparelho geniturinário</t>
+  </si>
+  <si>
+    <t>Doenças do aparelho respiratório</t>
+  </si>
+  <si>
+    <t>Doenças endócrinas, nutricionais e metabólicas</t>
+  </si>
+  <si>
+    <t>Neoplasmas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,6 +131,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -405,14 +421,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,270 +489,261 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>16</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>29</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>33</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>73</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>107</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>129</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>149</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>198</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>207</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>250</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>707</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>3</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>4</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3">
         <v>8</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3">
         <v>6</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3">
         <v>7</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P3">
         <v>10</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3">
         <v>33</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R3">
         <v>107</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>11</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>7</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>13</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>15</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>28</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>35</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4">
         <v>45</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4">
         <v>57</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4">
         <v>76</v>
       </c>
-      <c r="P4" t="n">
+      <c r="P4">
         <v>111</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4">
         <v>133</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4">
         <v>458</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" t="n">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>12</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5">
         <v>13</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5">
         <v>20</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5">
         <v>18</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5">
         <v>27</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P5">
         <v>35</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5">
         <v>41</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R5">
         <v>94</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>8</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>11</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>17</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>35</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>52</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6">
         <v>106</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6">
         <v>112</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6">
         <v>150</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6">
         <v>164</v>
       </c>
-      <c r="P6" t="n">
+      <c r="P6">
         <v>170</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6">
         <v>147</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6">
         <v>283</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>